<commit_message>
Nema NULL vrednosti u Excel-u!
</commit_message>
<xml_diff>
--- a/Schema_Workbench/Reservations.xlsx
+++ b/Schema_Workbench/Reservations.xlsx
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="187" r:id="rId2"/>
+    <pivotCache cacheId="43" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -211,14 +211,14 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Stefan Djukic" refreshedDate="44679.55251134259" backgroundQuery="1" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="0">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Stefan Djukic" refreshedDate="44683.834817129631" backgroundQuery="1" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="0">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="0"/>
   <cacheHierarchies count="10">
     <cacheHierarchy uniqueName="[Date.Default]" caption="Default" time="1" defaultMemberUniqueName="[Date.Default].[All Date.Defaults]" allUniqueName="[Date.Default].[All Date.Defaults]" dimensionUniqueName="[Date]" count="5" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Flight.Default]" caption="Default" defaultMemberUniqueName="[Flight.Default].[All Flight.Defaults]" allUniqueName="[Flight.Default].[All Flight.Defaults]" dimensionUniqueName="[Flight]" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Passanger.Default]" caption="Default" defaultMemberUniqueName="[Passanger.Default].[All Passanger.Defaults]" allUniqueName="[Passanger.Default].[All Passanger.Defaults]" dimensionUniqueName="[Passanger]" count="4" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Plane.Default]" caption="Default" defaultMemberUniqueName="[Plane.Default].[All Plane.Defaults]" allUniqueName="[Plane.Default].[All Plane.Defaults]" dimensionUniqueName="[Plane]" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Plane.Default]" caption="Default" defaultMemberUniqueName="[Plane.Default].[All Plane.Defaults]" allUniqueName="[Plane.Default].[All Plane.Defaults]" dimensionUniqueName="[Plane]" count="4" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Measures].[AverageCost]" caption="AverageCost" measure="1" displayFolder="" measureGroup="" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[FlightHours]" caption="FlightHours" measure="1" displayFolder="" measureGroup="" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[FlightNumber]" caption="FlightNumber" measure="1" displayFolder="" measureGroup="" count="0"/>
@@ -243,8 +243,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="187" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
-  <location ref="A1:C18" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="43" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+  <location ref="I1:K18" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
   <pivotHierarchies count="10">
     <pivotHierarchy/>
     <pivotHierarchy/>
@@ -529,106 +529,127 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="I1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="5" width="15.77734375" customWidth="1"/>
-    <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5546875" customWidth="1"/>
+    <col min="10" max="10" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5546875" customWidth="1"/>
+    <col min="12" max="13" width="10.77734375" customWidth="1"/>
+    <col min="14" max="14" width="4" customWidth="1"/>
+    <col min="15" max="15" width="9.6640625" customWidth="1"/>
+    <col min="16" max="16" width="7" customWidth="1"/>
+    <col min="17" max="17" width="10.77734375" customWidth="1"/>
+    <col min="18" max="18" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.44140625" customWidth="1"/>
+    <col min="23" max="23" width="11.5546875" customWidth="1"/>
+    <col min="24" max="24" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="6"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="6"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="4"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="6"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="6"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="4"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="6"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="4"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="6"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="6"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="6"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="6"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="4"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="6"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="4"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="6"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="6"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="4"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="6"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="4"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="6"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="7"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="9"/>
+    <row r="1" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I1" s="1"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="3"/>
+    </row>
+    <row r="2" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I2" s="4"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="6"/>
+    </row>
+    <row r="3" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I3" s="4"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="6"/>
+    </row>
+    <row r="4" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I4" s="4"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="6"/>
+    </row>
+    <row r="5" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I5" s="4"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="6"/>
+    </row>
+    <row r="6" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I6" s="4"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="6"/>
+    </row>
+    <row r="7" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I7" s="4"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="6"/>
+    </row>
+    <row r="8" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I8" s="4"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="6"/>
+    </row>
+    <row r="9" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I9" s="4"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="6"/>
+    </row>
+    <row r="10" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I10" s="4"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="6"/>
+    </row>
+    <row r="11" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I11" s="4"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="6"/>
+    </row>
+    <row r="12" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I12" s="4"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="6"/>
+    </row>
+    <row r="13" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I13" s="4"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="6"/>
+    </row>
+    <row r="14" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I14" s="4"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="6"/>
+    </row>
+    <row r="15" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I15" s="4"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="6"/>
+    </row>
+    <row r="16" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I16" s="4"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="6"/>
+    </row>
+    <row r="17" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I17" s="4"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="6"/>
+    </row>
+    <row r="18" spans="9:11" x14ac:dyDescent="0.3">
+      <c r="I18" s="7"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>